<commit_message>
Inte mycket kvar på sprintarna som finns kvar, jag tror jag kommer lägga till några extra sprintar sen
</commit_message>
<xml_diff>
--- a/Sprint Backlog and Burndown - 2.xlsx
+++ b/Sprint Backlog and Burndown - 2.xlsx
@@ -434,7 +434,7 @@
   <dimension ref="B2:P37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -514,7 +514,9 @@
       <c r="M5">
         <v>0</v>
       </c>
-      <c r="N5" s="4"/>
+      <c r="N5" s="4">
+        <v>7</v>
+      </c>
       <c r="O5" s="4"/>
       <c r="P5" t="s">
         <v>1</v>
@@ -528,7 +530,7 @@
         <v>2</v>
       </c>
       <c r="J6">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="K6">
         <v>1</v>
@@ -553,7 +555,7 @@
         <v>3</v>
       </c>
       <c r="J7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K7">
         <v>1</v>
@@ -604,7 +606,7 @@
         <v>18</v>
       </c>
       <c r="J9">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="K9">
         <v>4</v>

</xml_diff>

<commit_message>
Klar med sprintarna som finns så jag kommer lägga in några imorgon och använda den övriga tiden på dom.
</commit_message>
<xml_diff>
--- a/Sprint Backlog and Burndown - 2.xlsx
+++ b/Sprint Backlog and Burndown - 2.xlsx
@@ -434,7 +434,7 @@
   <dimension ref="B2:P37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q12" sqref="Q12"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -536,12 +536,14 @@
         <v>1</v>
       </c>
       <c r="L6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M6">
         <v>0</v>
       </c>
-      <c r="N6" s="4"/>
+      <c r="N6" s="4">
+        <v>4</v>
+      </c>
       <c r="O6" s="4"/>
       <c r="P6" s="2" t="s">
         <v>2</v>
@@ -586,7 +588,7 @@
         <v>2</v>
       </c>
       <c r="L8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M8">
         <v>0</v>
@@ -612,7 +614,7 @@
         <v>4</v>
       </c>
       <c r="L9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M9">
         <v>0</v>

</xml_diff>